<commit_message>
20171213 修正Google Excel問題單 第78 79 81 83條
</commit_message>
<xml_diff>
--- a/templates/中班歷史查詢結果.xlsx
+++ b/templates/中班歷史查詢結果.xlsx
@@ -24,29 +24,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>行家</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>航班</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>主號</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>起運國別</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${table:data.OL_FLIGHTNO}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>${table:data.OL_IMPORTDT_EX}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>${table:data.CO_NAME}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>報機單(袋數)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>進口日期</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>行家</t>
+    <t>報機日期</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉貨(袋數)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>航班</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>主號</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>起運國別</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>${table:data.OL_FLIGHTNO}</t>
+    <t>${table:data.OL_REAL_IMPORTDT_EX}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -54,15 +82,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>${table:data.OL_IMPORTDT_EX}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>${table:data.CO_NAME}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>報機單(袋數)</t>
+    <t>${table:data.OL_COUNT}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>${table:data.OL_PULL_COUNT}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -70,7 +94,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>${table:data.OL_COUNT}</t>
+    <t>${table:data.OL_REASON}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -90,13 +114,11 @@
     <font>
       <sz val="12"/>
       <name val="宋体"/>
-      <charset val="136"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="宋体"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="9"/>
@@ -108,7 +130,6 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <charset val="136"/>
     </font>
     <font>
       <b/>
@@ -177,7 +198,23 @@
     <cellStyle name="3232" xfId="1"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -462,63 +499,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
     <col min="4" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="11.375" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:9" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B1">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>AND(COUNTIF($B$5:$B$62731,B1)+COUNTIF($B$1:$B$4,B1)&gt;1,NOT(ISBLANK(B1)))</formula>
+  <conditionalFormatting sqref="C1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>AND(COUNTIF($C$5:$C$62731,C1)+COUNTIF($C$1:$C$4,C1)&gt;1,NOT(ISBLANK(C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>